<commit_message>
Add alpha fold prediction and figure work
</commit_message>
<xml_diff>
--- a/Figure 1/Fig1 Data.xlsx
+++ b/Figure 1/Fig1 Data.xlsx
@@ -47533,7 +47533,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47652,7 +47652,7 @@
         <v>509</v>
       </c>
       <c r="C12" s="118" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D12" s="105"/>
     </row>
@@ -47662,7 +47662,7 @@
         <v>510</v>
       </c>
       <c r="C13" s="122" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="D13" s="105"/>
     </row>

</xml_diff>